<commit_message>
Date formulas and Concatenate info added
</commit_message>
<xml_diff>
--- a/Excel/Excel Assignment VLookup,IF,Pivot Table.xlsx
+++ b/Excel/Excel Assignment VLookup,IF,Pivot Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kishan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kishan\Desktop\Bootcamp.Info\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439255B7-1FA6-4093-B6C5-86675AAB8331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7FF926-D3A2-4404-BE9F-62C480525856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{062685F1-8DA9-460B-92B7-93046D225DE7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{062685F1-8DA9-460B-92B7-93046D225DE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock Ticker" sheetId="5" r:id="rId1"/>
@@ -19,9 +19,12 @@
     <sheet name="IF Function" sheetId="2" r:id="rId4"/>
     <sheet name="Pivot Table" sheetId="7" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'IF Function'!$A$1:$T$36</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="84">
   <si>
     <t>GOOG</t>
   </si>
@@ -287,6 +290,12 @@
   </si>
   <si>
     <t>Column Labels</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Stocks and days where Opening&gt;Close</t>
   </si>
 </sst>
 </file>
@@ -294,7 +303,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -333,18 +342,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,7 +413,7 @@
     <cacheField name="Open2" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="39.060001" maxValue="3402.1000979999999"/>
     </cacheField>
-    <cacheField name="Date" numFmtId="165">
+    <cacheField name="Date" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2021-10-26T00:00:00" maxDate="2021-11-02T00:00:00" count="5">
         <d v="2021-10-26T00:00:00"/>
         <d v="2021-10-27T00:00:00"/>
@@ -847,7 +857,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{55A7C059-B373-4EC0-A4EB-F653363202C3}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{55A7C059-B373-4EC0-A4EB-F653363202C3}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -870,7 +880,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" numFmtId="165" showAll="0">
+    <pivotField axis="axisCol" numFmtId="164" showAll="0">
       <items count="6">
         <item x="0"/>
         <item x="1"/>
@@ -1392,7 +1402,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1403,7 +1413,7 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D1" t="s">
@@ -1432,7 +1442,7 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>44495</v>
       </c>
       <c r="D2">
@@ -1461,7 +1471,7 @@
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>44496</v>
       </c>
       <c r="D3">
@@ -1490,7 +1500,7 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>44497</v>
       </c>
       <c r="D4">
@@ -1519,7 +1529,7 @@
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>44498</v>
       </c>
       <c r="D5">
@@ -1548,7 +1558,7 @@
       <c r="B6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>44501</v>
       </c>
       <c r="D6">
@@ -1577,7 +1587,7 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>44495</v>
       </c>
       <c r="D7">
@@ -1606,7 +1616,7 @@
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>44496</v>
       </c>
       <c r="D8">
@@ -1635,7 +1645,7 @@
       <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>44497</v>
       </c>
       <c r="D9">
@@ -1664,7 +1674,7 @@
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>44498</v>
       </c>
       <c r="D10">
@@ -1693,7 +1703,7 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>44501</v>
       </c>
       <c r="D11">
@@ -1722,7 +1732,7 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>44495</v>
       </c>
       <c r="D12">
@@ -1751,7 +1761,7 @@
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>44496</v>
       </c>
       <c r="D13">
@@ -1780,7 +1790,7 @@
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>44497</v>
       </c>
       <c r="D14">
@@ -1809,7 +1819,7 @@
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>44498</v>
       </c>
       <c r="D15">
@@ -1838,7 +1848,7 @@
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>44501</v>
       </c>
       <c r="D16">
@@ -1867,7 +1877,7 @@
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>44495</v>
       </c>
       <c r="D17">
@@ -1896,7 +1906,7 @@
       <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>44496</v>
       </c>
       <c r="D18">
@@ -1925,7 +1935,7 @@
       <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>44497</v>
       </c>
       <c r="D19">
@@ -1954,7 +1964,7 @@
       <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>44498</v>
       </c>
       <c r="D20">
@@ -1983,7 +1993,7 @@
       <c r="B21" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>44501</v>
       </c>
       <c r="D21">
@@ -2012,7 +2022,7 @@
       <c r="B22" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>44495</v>
       </c>
       <c r="D22">
@@ -2041,7 +2051,7 @@
       <c r="B23" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>44496</v>
       </c>
       <c r="D23">
@@ -2070,7 +2080,7 @@
       <c r="B24" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>44497</v>
       </c>
       <c r="D24">
@@ -2099,7 +2109,7 @@
       <c r="B25" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>44498</v>
       </c>
       <c r="D25">
@@ -2128,7 +2138,7 @@
       <c r="B26" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>44501</v>
       </c>
       <c r="D26">
@@ -2157,7 +2167,7 @@
       <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>44495</v>
       </c>
       <c r="D27">
@@ -2186,7 +2196,7 @@
       <c r="B28" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>44496</v>
       </c>
       <c r="D28">
@@ -2215,7 +2225,7 @@
       <c r="B29" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>44497</v>
       </c>
       <c r="D29">
@@ -2244,7 +2254,7 @@
       <c r="B30" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>44498</v>
       </c>
       <c r="D30">
@@ -2273,7 +2283,7 @@
       <c r="B31" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>44501</v>
       </c>
       <c r="D31">
@@ -2302,7 +2312,7 @@
       <c r="B32" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>44495</v>
       </c>
       <c r="D32">
@@ -2331,7 +2341,7 @@
       <c r="B33" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>44496</v>
       </c>
       <c r="D33">
@@ -2360,7 +2370,7 @@
       <c r="B34" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>44497</v>
       </c>
       <c r="D34">
@@ -2389,7 +2399,7 @@
       <c r="B35" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>44498</v>
       </c>
       <c r="D35">
@@ -2418,7 +2428,7 @@
       <c r="B36" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>44501</v>
       </c>
       <c r="D36">
@@ -2451,7 +2461,7 @@
   <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2528,19 +2538,19 @@
         <f>VLOOKUP(A2,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>2780.110107</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <f>VLOOKUP(A2,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2578,17 +2588,17 @@
         <f>VLOOKUP(A3,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>38.909999999999997</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <f>VLOOKUP(A3,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -2626,17 +2636,17 @@
         <f>VLOOKUP(A4,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>82.279999000000004</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <f>VLOOKUP(A4,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2674,17 +2684,17 @@
         <f>VLOOKUP(A5,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>39.459999000000003</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <f>VLOOKUP(A5,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -2722,17 +2732,17 @@
         <f>VLOOKUP(A6,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>46.759998000000003</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <f>VLOOKUP(A6,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2770,17 +2780,17 @@
         <f>VLOOKUP(A7,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>3386</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <f>VLOOKUP(A7,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -2818,17 +2828,17 @@
         <f>VLOOKUP(A8,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>46.509998000000003</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <f>VLOOKUP(A8,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -2866,7 +2876,7 @@
         <f>VLOOKUP(A9,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>85.169998000000007</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <f>VLOOKUP(A9,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
@@ -2907,7 +2917,7 @@
         <f>VLOOKUP(A10,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>96</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <f>VLOOKUP(A10,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
@@ -2948,7 +2958,7 @@
         <f>VLOOKUP(A11,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>95.459998999999996</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <f>VLOOKUP(A11,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
@@ -2989,7 +2999,7 @@
         <f>VLOOKUP(A12,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>149.720001</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <f>VLOOKUP(A12,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
@@ -3030,7 +3040,7 @@
         <f>VLOOKUP(A13,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>3343.9799800000001</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <f>VLOOKUP(A13,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
@@ -3071,7 +3081,7 @@
         <f>VLOOKUP(A14,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>38.830002</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <f>VLOOKUP(A14,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
@@ -3112,7 +3122,7 @@
         <f>VLOOKUP(A15,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>46.439999</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <f>VLOOKUP(A15,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
@@ -3153,7 +3163,7 @@
         <f>VLOOKUP(A16,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>93.910004000000001</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <f>VLOOKUP(A16,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
@@ -3194,7 +3204,7 @@
         <f>VLOOKUP(A17,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>47.060001</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="2">
         <f>VLOOKUP(A17,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
@@ -3235,7 +3245,7 @@
         <f>VLOOKUP(A18,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>85.360000999999997</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <f>VLOOKUP(A18,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
@@ -3276,7 +3286,7 @@
         <f>VLOOKUP(A19,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>84.150002000000001</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <f>VLOOKUP(A19,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
@@ -3317,7 +3327,7 @@
         <f>VLOOKUP(A20,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>149.009995</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <f>VLOOKUP(A20,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
@@ -3358,7 +3368,7 @@
         <f>VLOOKUP(A21,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>146.41000399999999</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <f>VLOOKUP(A21,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
@@ -3399,7 +3409,7 @@
         <f>VLOOKUP(A22,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>2798.0500489999999</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <f>VLOOKUP(A22,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
@@ -3440,7 +3450,7 @@
         <f>VLOOKUP(A23,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>148.490005</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <f>VLOOKUP(A23,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
@@ -3481,7 +3491,7 @@
         <f>VLOOKUP(A24,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>3273.320068</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="2">
         <f>VLOOKUP(A24,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
@@ -3522,7 +3532,7 @@
         <f>VLOOKUP(A25,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>2903.330078</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="2">
         <f>VLOOKUP(A25,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
@@ -3563,7 +3573,7 @@
         <f>VLOOKUP(A26,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>2895.2700199999999</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="2">
         <f>VLOOKUP(A26,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
@@ -3604,7 +3614,7 @@
         <f>VLOOKUP(A27,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>147.800003</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="2">
         <f>VLOOKUP(A27,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
@@ -3645,7 +3655,7 @@
         <f>VLOOKUP(A28,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>95.93</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="2">
         <f>VLOOKUP(A28,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
@@ -3686,7 +3696,7 @@
         <f>VLOOKUP(A29,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>82.699996999999996</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="2">
         <f>VLOOKUP(A29,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
@@ -3727,7 +3737,7 @@
         <f>VLOOKUP(A30,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>96.940002000000007</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="2">
         <f>VLOOKUP(A30,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
@@ -3768,7 +3778,7 @@
         <f>VLOOKUP(A31,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>47.32</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="2">
         <f>VLOOKUP(A31,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
@@ -3809,7 +3819,7 @@
         <f>VLOOKUP(A32,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>3292.0200199999999</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="2">
         <f>VLOOKUP(A32,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
@@ -3850,7 +3860,7 @@
         <f>VLOOKUP(A33,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>39.020000000000003</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="2">
         <f>VLOOKUP(A33,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
@@ -3891,7 +3901,7 @@
         <f>VLOOKUP(A34,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>3371.4499510000001</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="2">
         <f>VLOOKUP(A34,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
@@ -3932,7 +3942,7 @@
         <f>VLOOKUP(A35,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>2871.5900879999999</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="2">
         <f>VLOOKUP(A35,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
@@ -3973,7 +3983,7 @@
         <f>VLOOKUP(A36,'Stock Data'!$A$2:$F$36,6,FALSE)</f>
         <v>38.810001</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="2">
         <f>VLOOKUP(A36,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
@@ -3988,21 +3998,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602863BD-0A20-4C8B-96CF-B4D07A018C29}">
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="3"/>
+    <col min="10" max="10" width="8.88671875" style="2"/>
     <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -4030,14 +4040,14 @@
       <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -4073,7 +4083,7 @@
         <f>VLOOKUP(A2,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>2812.1201169999999</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <f>VLOOKUP(A2,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
@@ -4082,7 +4092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -4118,25 +4128,25 @@
         <f>VLOOKUP(A3,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>2798.0500489999999</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <f>VLOOKUP(A3,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K36" si="0">IF(I3&gt;F3,"1","o")</f>
+        <f>IF(I3&gt;F3,"1","o")</f>
         <v>o</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -4172,23 +4182,23 @@
         <f>VLOOKUP(A4,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>2945.9799800000001</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <f>VLOOKUP(A4,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I4&gt;F4,"1","o")</f>
         <v>1</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -4224,23 +4234,23 @@
         <f>VLOOKUP(A5,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>2910.3999020000001</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <f>VLOOKUP(A5,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I5&gt;F5,"1","o")</f>
         <v>o</v>
       </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -4276,23 +4286,23 @@
         <f>VLOOKUP(A6,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>2963.3000489999999</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <f>VLOOKUP(A6,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I6&gt;F6,"1","o")</f>
         <v>1</v>
       </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -4328,23 +4338,23 @@
         <f>VLOOKUP(A7,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>149.33000200000001</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <f>VLOOKUP(A7,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I7&gt;F7,"1","o")</f>
         <v>1</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -4380,23 +4390,23 @@
         <f>VLOOKUP(A8,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>149.36000100000001</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <f>VLOOKUP(A8,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I8&gt;F8,"1","o")</f>
         <v>1</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -4432,23 +4442,23 @@
         <f>VLOOKUP(A9,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>149.820007</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <f>VLOOKUP(A9,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I9&gt;F9,"1","o")</f>
         <v>o</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -4484,16 +4494,16 @@
         <f>VLOOKUP(A10,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>147.220001</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <f>VLOOKUP(A10,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I10&gt;F10,"1","o")</f>
         <v>o</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -4529,16 +4539,16 @@
         <f>VLOOKUP(A11,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>148.990005</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <f>VLOOKUP(A11,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I11&gt;F11,"1","o")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -4574,16 +4584,19 @@
         <f>VLOOKUP(A12,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>3349.51001</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <f>VLOOKUP(A12,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I12&gt;F12,"1","o")</f>
         <v>o</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N12" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -4619,16 +4632,49 @@
         <f>VLOOKUP(A13,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>3388</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <f>VLOOKUP(A13,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I13&gt;F13,"1","o")</f>
         <v>o</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>2812.1201169999999</v>
+      </c>
+      <c r="R13">
+        <v>2793.4399410000001</v>
+      </c>
+      <c r="S13">
+        <v>2793.4399410000001</v>
+      </c>
+      <c r="T13">
+        <v>2816.790039</v>
+      </c>
+      <c r="U13">
+        <v>2780.110107</v>
+      </c>
+      <c r="V13">
+        <v>2812.1201169999999</v>
+      </c>
+      <c r="W13" s="2">
+        <v>44495</v>
+      </c>
+      <c r="X13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -4664,16 +4710,49 @@
         <f>VLOOKUP(A14,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>3402.1000979999999</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <f>VLOOKUP(A14,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I14&gt;F14,"1","o")</f>
         <v>o</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>2945.9799800000001</v>
+      </c>
+      <c r="R14">
+        <v>2922.580078</v>
+      </c>
+      <c r="S14">
+        <v>2922.580078</v>
+      </c>
+      <c r="T14">
+        <v>2948.48999</v>
+      </c>
+      <c r="U14">
+        <v>2895.2700199999999</v>
+      </c>
+      <c r="V14">
+        <v>2945.9799800000001</v>
+      </c>
+      <c r="W14" s="2">
+        <v>44497</v>
+      </c>
+      <c r="X14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -4709,16 +4788,49 @@
         <f>VLOOKUP(A15,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>3300.0200199999999</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <f>VLOOKUP(A15,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I15&gt;F15,"1","o")</f>
         <v>o</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>2963.3000489999999</v>
+      </c>
+      <c r="R15">
+        <v>2875.4799800000001</v>
+      </c>
+      <c r="S15">
+        <v>2875.4799800000001</v>
+      </c>
+      <c r="T15">
+        <v>2967.98999</v>
+      </c>
+      <c r="U15">
+        <v>2871.5900879999999</v>
+      </c>
+      <c r="V15">
+        <v>2963.3000489999999</v>
+      </c>
+      <c r="W15" s="2">
+        <v>44501</v>
+      </c>
+      <c r="X15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -4754,16 +4866,49 @@
         <f>VLOOKUP(A16,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>3361.8000489999999</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <f>VLOOKUP(A16,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I16&gt;F16,"1","o")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O16" t="s">
+        <v>4</v>
+      </c>
+      <c r="P16" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16">
+        <v>149.33000200000001</v>
+      </c>
+      <c r="R16">
+        <v>149.320007</v>
+      </c>
+      <c r="S16">
+        <v>149.320007</v>
+      </c>
+      <c r="T16">
+        <v>150.83999600000001</v>
+      </c>
+      <c r="U16">
+        <v>149.009995</v>
+      </c>
+      <c r="V16">
+        <v>149.33000200000001</v>
+      </c>
+      <c r="W16" s="2">
+        <v>44495</v>
+      </c>
+      <c r="X16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
@@ -4799,16 +4944,49 @@
         <f>VLOOKUP(A17,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>39.909999999999997</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="2">
         <f>VLOOKUP(A17,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I17&gt;F17,"1","o")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P17" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17">
+        <v>149.36000100000001</v>
+      </c>
+      <c r="R17">
+        <v>148.85000600000001</v>
+      </c>
+      <c r="S17">
+        <v>148.85000600000001</v>
+      </c>
+      <c r="T17">
+        <v>149.729996</v>
+      </c>
+      <c r="U17">
+        <v>148.490005</v>
+      </c>
+      <c r="V17">
+        <v>149.36000100000001</v>
+      </c>
+      <c r="W17" s="2">
+        <v>44496</v>
+      </c>
+      <c r="X17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
@@ -4844,16 +5022,49 @@
         <f>VLOOKUP(A18,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>39.840000000000003</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <f>VLOOKUP(A18,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I18&gt;F18,"1","o")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O18" t="s">
+        <v>4</v>
+      </c>
+      <c r="P18" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q18">
+        <v>148.990005</v>
+      </c>
+      <c r="R18">
+        <v>148.96000699999999</v>
+      </c>
+      <c r="S18">
+        <v>148.96000699999999</v>
+      </c>
+      <c r="T18">
+        <v>149.699997</v>
+      </c>
+      <c r="U18">
+        <v>147.800003</v>
+      </c>
+      <c r="V18">
+        <v>148.990005</v>
+      </c>
+      <c r="W18" s="2">
+        <v>44501</v>
+      </c>
+      <c r="X18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -4889,16 +5100,49 @@
         <f>VLOOKUP(A19,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>39.139999000000003</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <f>VLOOKUP(A19,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I19&gt;F19,"1","o")</f>
         <v>o</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O19" t="s">
+        <v>7</v>
+      </c>
+      <c r="P19" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q19">
+        <v>3361.8000489999999</v>
+      </c>
+      <c r="R19">
+        <v>3318.110107</v>
+      </c>
+      <c r="S19">
+        <v>3318.110107</v>
+      </c>
+      <c r="T19">
+        <v>3375.860107</v>
+      </c>
+      <c r="U19">
+        <v>3292.0200199999999</v>
+      </c>
+      <c r="V19">
+        <v>3361.8000489999999</v>
+      </c>
+      <c r="W19" s="2">
+        <v>44501</v>
+      </c>
+      <c r="X19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
@@ -4934,16 +5178,49 @@
         <f>VLOOKUP(A20,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>39.060001</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <f>VLOOKUP(A20,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I20&gt;F20,"1","o")</f>
         <v>o</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O20" t="s">
+        <v>14</v>
+      </c>
+      <c r="P20" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q20">
+        <v>39.909999999999997</v>
+      </c>
+      <c r="R20">
+        <v>39.709999000000003</v>
+      </c>
+      <c r="S20">
+        <v>39.709999000000003</v>
+      </c>
+      <c r="T20">
+        <v>40.290000999999997</v>
+      </c>
+      <c r="U20">
+        <v>39.459999000000003</v>
+      </c>
+      <c r="V20">
+        <v>39.909999999999997</v>
+      </c>
+      <c r="W20" s="2">
+        <v>44495</v>
+      </c>
+      <c r="X20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
@@ -4979,16 +5256,49 @@
         <f>VLOOKUP(A21,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>39.150002000000001</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <f>VLOOKUP(A21,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I21&gt;F21,"1","o")</f>
         <v>o</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O21" t="s">
+        <v>14</v>
+      </c>
+      <c r="P21" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q21">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="R21">
+        <v>39.07</v>
+      </c>
+      <c r="S21">
+        <v>39.07</v>
+      </c>
+      <c r="T21">
+        <v>39.93</v>
+      </c>
+      <c r="U21">
+        <v>39.020000000000003</v>
+      </c>
+      <c r="V21">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="W21" s="2">
+        <v>44496</v>
+      </c>
+      <c r="X21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
@@ -5024,16 +5334,49 @@
         <f>VLOOKUP(A22,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>48</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <f>VLOOKUP(A22,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I22&gt;F22,"1","o")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P22" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q22">
+        <v>48</v>
+      </c>
+      <c r="R22">
+        <v>47.59</v>
+      </c>
+      <c r="S22">
+        <v>47.59</v>
+      </c>
+      <c r="T22">
+        <v>48.150002000000001</v>
+      </c>
+      <c r="U22">
+        <v>47.32</v>
+      </c>
+      <c r="V22">
+        <v>48</v>
+      </c>
+      <c r="W22" s="2">
+        <v>44495</v>
+      </c>
+      <c r="X22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
@@ -5069,16 +5412,49 @@
         <f>VLOOKUP(A23,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>47.599997999999999</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <f>VLOOKUP(A23,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I23&gt;F23,"1","o")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O23" t="s">
+        <v>16</v>
+      </c>
+      <c r="P23" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q23">
+        <v>47.599997999999999</v>
+      </c>
+      <c r="R23">
+        <v>46.57</v>
+      </c>
+      <c r="S23">
+        <v>46.57</v>
+      </c>
+      <c r="T23">
+        <v>47.669998</v>
+      </c>
+      <c r="U23">
+        <v>46.509998000000003</v>
+      </c>
+      <c r="V23">
+        <v>47.599997999999999</v>
+      </c>
+      <c r="W23" s="2">
+        <v>44496</v>
+      </c>
+      <c r="X23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -5114,16 +5490,49 @@
         <f>VLOOKUP(A24,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>46.529998999999997</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="2">
         <f>VLOOKUP(A24,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I24&gt;F24,"1","o")</f>
         <v>o</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O24" t="s">
+        <v>12</v>
+      </c>
+      <c r="P24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q24">
+        <v>98.300003000000004</v>
+      </c>
+      <c r="R24">
+        <v>96.980002999999996</v>
+      </c>
+      <c r="S24">
+        <v>96.980002999999996</v>
+      </c>
+      <c r="T24">
+        <v>98.559997999999993</v>
+      </c>
+      <c r="U24">
+        <v>96.940002000000007</v>
+      </c>
+      <c r="V24">
+        <v>98.300003000000004</v>
+      </c>
+      <c r="W24" s="2">
+        <v>44495</v>
+      </c>
+      <c r="X24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
@@ -5159,16 +5568,49 @@
         <f>VLOOKUP(A25,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>47.02</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="2">
         <f>VLOOKUP(A25,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I25&gt;F25,"1","o")</f>
         <v>o</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O25" t="s">
+        <v>12</v>
+      </c>
+      <c r="P25" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q25">
+        <v>96.809997999999993</v>
+      </c>
+      <c r="R25">
+        <v>96.029999000000004</v>
+      </c>
+      <c r="S25">
+        <v>96.029999000000004</v>
+      </c>
+      <c r="T25">
+        <v>97.300003000000004</v>
+      </c>
+      <c r="U25">
+        <v>96</v>
+      </c>
+      <c r="V25">
+        <v>96.809997999999993</v>
+      </c>
+      <c r="W25" s="2">
+        <v>44496</v>
+      </c>
+      <c r="X25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>62</v>
       </c>
@@ -5204,16 +5646,49 @@
         <f>VLOOKUP(A26,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>47.34</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="2">
         <f>VLOOKUP(A26,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I26&gt;F26,"1","o")</f>
         <v>o</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O26" t="s">
+        <v>12</v>
+      </c>
+      <c r="P26" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q26">
+        <v>96.650002000000001</v>
+      </c>
+      <c r="R26">
+        <v>96.230002999999996</v>
+      </c>
+      <c r="S26">
+        <v>96.230002999999996</v>
+      </c>
+      <c r="T26">
+        <v>97.699996999999996</v>
+      </c>
+      <c r="U26">
+        <v>95.93</v>
+      </c>
+      <c r="V26">
+        <v>96.650002000000001</v>
+      </c>
+      <c r="W26" s="2">
+        <v>44497</v>
+      </c>
+      <c r="X26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>63</v>
       </c>
@@ -5249,16 +5724,49 @@
         <f>VLOOKUP(A27,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>98.300003000000004</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="2">
         <f>VLOOKUP(A27,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I27&gt;F27,"1","o")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O27" t="s">
+        <v>12</v>
+      </c>
+      <c r="P27" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q27">
+        <v>96</v>
+      </c>
+      <c r="R27">
+        <v>94.379997000000003</v>
+      </c>
+      <c r="S27">
+        <v>94.379997000000003</v>
+      </c>
+      <c r="T27">
+        <v>96.029999000000004</v>
+      </c>
+      <c r="U27">
+        <v>93.910004000000001</v>
+      </c>
+      <c r="V27">
+        <v>96</v>
+      </c>
+      <c r="W27" s="2">
+        <v>44501</v>
+      </c>
+      <c r="X27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
@@ -5294,16 +5802,49 @@
         <f>VLOOKUP(A28,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>96.809997999999993</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="2">
         <f>VLOOKUP(A28,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I28&gt;F28,"1","o")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O28" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q28">
+        <v>84.160004000000001</v>
+      </c>
+      <c r="R28">
+        <v>83.040001000000004</v>
+      </c>
+      <c r="S28">
+        <v>83.040001000000004</v>
+      </c>
+      <c r="T28">
+        <v>84.730002999999996</v>
+      </c>
+      <c r="U28">
+        <v>82.699996999999996</v>
+      </c>
+      <c r="V28">
+        <v>84.160004000000001</v>
+      </c>
+      <c r="W28" s="2">
+        <v>44495</v>
+      </c>
+      <c r="X28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -5339,16 +5880,49 @@
         <f>VLOOKUP(A29,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>96.650002000000001</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="2">
         <f>VLOOKUP(A29,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I29&gt;F29,"1","o")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O29" t="s">
+        <v>24</v>
+      </c>
+      <c r="P29" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q29">
+        <v>86.029999000000004</v>
+      </c>
+      <c r="R29">
+        <v>85.400002000000001</v>
+      </c>
+      <c r="S29">
+        <v>85.400002000000001</v>
+      </c>
+      <c r="T29">
+        <v>87.239998</v>
+      </c>
+      <c r="U29">
+        <v>85.360000999999997</v>
+      </c>
+      <c r="V29">
+        <v>86.029999000000004</v>
+      </c>
+      <c r="W29" s="2">
+        <v>44497</v>
+      </c>
+      <c r="X29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
@@ -5384,16 +5958,16 @@
         <f>VLOOKUP(A30,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>95.790001000000004</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="2">
         <f>VLOOKUP(A30,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I30&gt;F30,"1","o")</f>
         <v>o</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
@@ -5429,16 +6003,16 @@
         <f>VLOOKUP(A31,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>96</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="2">
         <f>VLOOKUP(A31,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I31&gt;F31,"1","o")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>68</v>
       </c>
@@ -5474,12 +6048,12 @@
         <f>VLOOKUP(A32,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>84.160004000000001</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="2">
         <f>VLOOKUP(A32,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44495</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I32&gt;F32,"1","o")</f>
         <v>1</v>
       </c>
     </row>
@@ -5519,12 +6093,12 @@
         <f>VLOOKUP(A33,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>82.669998000000007</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="2">
         <f>VLOOKUP(A33,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44496</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I33&gt;F33,"1","o")</f>
         <v>o</v>
       </c>
     </row>
@@ -5564,12 +6138,12 @@
         <f>VLOOKUP(A34,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>86.029999000000004</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="2">
         <f>VLOOKUP(A34,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44497</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(I34&gt;F34,"1","o")</f>
         <v>1</v>
       </c>
     </row>
@@ -5609,12 +6183,12 @@
         <f>VLOOKUP(A35,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>84.919998000000007</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="2">
         <f>VLOOKUP(A35,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44498</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K35:K36" si="0">IF(I35&gt;F35,"1","o")</f>
         <v>o</v>
       </c>
     </row>
@@ -5654,7 +6228,7 @@
         <f>VLOOKUP(A36,'Stock Data'!$A$2:$D$36,4,FALSE)</f>
         <v>85.449996999999996</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="2">
         <f>VLOOKUP(A36,'Stock Data'!$A$2:$C$36,3,FALSE)</f>
         <v>44501</v>
       </c>
@@ -5664,6 +6238,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:T36" xr:uid="{602863BD-0A20-4C8B-96CF-B4D07A018C29}"/>
   <mergeCells count="1">
     <mergeCell ref="N3:T9"/>
   </mergeCells>
@@ -5675,8 +6250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92996C93-B40E-42DE-8EA2-D3887BE8450E}">
   <dimension ref="A2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:M26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5692,284 +6267,284 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>44495</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>44496</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>44497</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>44498</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>44501</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>3349.51001</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>3388</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>3402.1000979999999</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>3300.0200199999999</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>3361.8000489999999</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>3360.2860354000004</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>149.33000200000001</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>149.36000100000001</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>149.820007</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>147.220001</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>148.990005</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>148.94400320000003</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>39.909999999999997</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>39.840000000000003</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>39.139999000000003</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>39.060001</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>39.150002000000001</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>39.420000399999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>2812.1201169999999</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>2798.0500489999999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>2945.9799800000001</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>2910.3999020000001</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>2963.3000489999999</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>2885.9700194000002</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>84.160004000000001</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>82.669998000000007</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>86.029999000000004</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>84.919998000000007</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>85.449996999999996</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>84.645999200000006</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>98.300003000000004</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>96.809997999999993</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>96.650002000000001</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>95.790001000000004</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>96</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>96.710000800000003</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>48</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>47.599997999999999</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>46.529998999999997</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>47.02</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>47.34</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>47.297999400000002</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>940.19001942857153</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>943.19000628571428</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>966.60715485714297</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>946.34713185714304</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>963.1471574285714</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>951.89629397142858</v>
       </c>
     </row>
     <row r="20" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
     </row>
     <row r="22" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
     </row>
     <row r="23" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
     </row>
     <row r="24" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
     </row>
     <row r="25" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
     </row>
     <row r="26" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>